<commit_message>
SE and OP analysis from model available
</commit_message>
<xml_diff>
--- a/+iamd/+models/inputs2.xlsx
+++ b/+iamd/+models/inputs2.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\Purdue MSAA\SoS\Project\ABM\+iamd\+models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA17860-E2A8-4034-BCE1-311C37705D8D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9440C1F5-3B5F-4242-9D59-BB28F0196221}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="8040" xr2:uid="{E29C2BC3-3FA1-4886-8308-3CCAE90EA738}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="7350" tabRatio="442" activeTab="1" xr2:uid="{E29C2BC3-3FA1-4886-8308-3CCAE90EA738}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation" sheetId="1" r:id="rId1"/>
     <sheet name="Friendly" sheetId="2" r:id="rId2"/>
-    <sheet name="Threats" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Radar 1</t>
   </si>
@@ -53,21 +52,6 @@
     <t>Satellite 1</t>
   </si>
   <si>
-    <t>Starting Location</t>
-  </si>
-  <si>
-    <t>Destination</t>
-  </si>
-  <si>
-    <t>Missile 1</t>
-  </si>
-  <si>
-    <t>Missile 2</t>
-  </si>
-  <si>
-    <t>Time of launch</t>
-  </si>
-  <si>
     <t>z-coord</t>
   </si>
   <si>
@@ -80,9 +64,6 @@
     <t>Command 1</t>
   </si>
   <si>
-    <t>arsenal</t>
-  </si>
-  <si>
     <t>BATTERY</t>
   </si>
   <si>
@@ -95,20 +76,23 @@
     <t>Battery 3</t>
   </si>
   <si>
-    <t>Battery4</t>
-  </si>
-  <si>
     <t>Sim Start Time</t>
   </si>
   <si>
     <t>Sim End Time</t>
+  </si>
+  <si>
+    <t>Battery 4</t>
+  </si>
+  <si>
+    <t>Self-effectiveness (0-100)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,16 +108,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -141,25 +170,148 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC0000"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFCC99FF"/>
+      <color rgb="FFCC66FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -470,7 +622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21A8DF9-35E4-44AA-913D-9559ADD0E3C4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -482,10 +634,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -493,7 +645,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -506,354 +658,270 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF88F09-9BE8-4712-94BD-426562776ABE}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="24.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="9.140625" style="2"/>
+    <col min="13" max="13" width="24.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="2"/>
+    <col min="15" max="15" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="9.140625" style="2"/>
+    <col min="19" max="19" width="24.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="2"/>
+    <col min="21" max="21" width="9.140625" style="6"/>
+    <col min="22" max="25" width="9.140625" style="2"/>
+    <col min="26" max="26" width="24.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="F1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="K1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="M1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="R1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="X1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>17</v>
+      <c r="Z1" s="19" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9">
         <v>669</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="9">
         <v>121</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="9">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9">
         <v>250</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="20">
+        <v>100</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="9">
+        <v>0</v>
+      </c>
+      <c r="J2" s="9">
+        <v>500</v>
+      </c>
+      <c r="K2" s="9">
+        <v>0</v>
+      </c>
+      <c r="L2" s="9">
+        <v>500</v>
+      </c>
+      <c r="M2" s="20">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>500</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>500</v>
-      </c>
-      <c r="O2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2">
+      <c r="O2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="9">
         <v>733</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="9">
         <v>513</v>
       </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="U2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V2">
+      <c r="R2" s="9">
+        <v>0</v>
+      </c>
+      <c r="S2" s="20">
+        <v>100</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" s="9">
         <v>710</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="9">
         <v>94</v>
       </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
+      <c r="X2" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="9">
         <v>150</v>
       </c>
-      <c r="Z2">
-        <v>5</v>
+      <c r="Z2" s="20">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>483</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>371</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
         <v>250</v>
       </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="U3" t="s">
-        <v>20</v>
-      </c>
-      <c r="V3">
+      <c r="F3" s="21">
+        <v>100</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="V3" s="2">
         <v>558</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="2">
         <v>345</v>
       </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
+      <c r="X3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="2">
         <v>150</v>
       </c>
-      <c r="Z3">
-        <v>5</v>
+      <c r="Z3" s="20">
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>477</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>753</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
         <v>250</v>
       </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="U4" t="s">
-        <v>21</v>
-      </c>
-      <c r="V4">
+      <c r="F4" s="21">
+        <v>100</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V4" s="2">
         <v>495</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="2">
         <v>629</v>
       </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
+      <c r="X4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="2">
         <v>150</v>
       </c>
-      <c r="Z4">
-        <v>5</v>
+      <c r="Z4" s="20">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U5" t="s">
-        <v>22</v>
-      </c>
-      <c r="V5">
+      <c r="U5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="V5" s="2">
         <v>523</v>
       </c>
-      <c r="W5">
+      <c r="W5" s="2">
         <v>876</v>
       </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
+      <c r="X5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="2">
         <v>150</v>
       </c>
-      <c r="Z5">
-        <v>5</v>
+      <c r="Z5" s="20">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54476DE5-86B1-4500-81D3-7C85006101D6}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1000</v>
-      </c>
-      <c r="F3">
-        <v>1000</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1000</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1000</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
model ready for OP runs
</commit_message>
<xml_diff>
--- a/+iamd/+models/inputs2.xlsx
+++ b/+iamd/+models/inputs2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\Purdue MSAA\SoS\Project\ABM\+iamd\+models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9440C1F5-3B5F-4242-9D59-BB28F0196221}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD979E25-131A-4EB4-A82B-EF75FF39AF72}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="7350" tabRatio="442" activeTab="1" xr2:uid="{E29C2BC3-3FA1-4886-8308-3CCAE90EA738}"/>
   </bookViews>
@@ -275,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -297,7 +297,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,7 +622,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF88F09-9BE8-4712-94BD-426562776ABE}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -788,7 +787,7 @@
         <v>500</v>
       </c>
       <c r="M2" s="20">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="O2" s="15" t="s">
         <v>11</v>
@@ -840,7 +839,7 @@
       <c r="E3" s="2">
         <v>250</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="20">
         <v>100</v>
       </c>
       <c r="U3" s="6" t="s">
@@ -878,7 +877,7 @@
       <c r="E4" s="2">
         <v>250</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="20">
         <v>100</v>
       </c>
       <c r="U4" s="6" t="s">

</xml_diff>

<commit_message>
now outputs time to detect, assign, num intercepts, num cues to a text file which is continually appended for each trial
</commit_message>
<xml_diff>
--- a/+iamd/+models/inputs2.xlsx
+++ b/+iamd/+models/inputs2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\Purdue MSAA\SoS\Project\ABM\+iamd\+models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD979E25-131A-4EB4-A82B-EF75FF39AF72}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8A143C-4B95-4448-A34E-57B34A2F62C3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="7350" tabRatio="442" activeTab="1" xr2:uid="{E29C2BC3-3FA1-4886-8308-3CCAE90EA738}"/>
   </bookViews>
@@ -622,7 +622,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -657,7 +657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF88F09-9BE8-4712-94BD-426562776ABE}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
quicker data collection: runner file that loops from SE from 0 to 90
</commit_message>
<xml_diff>
--- a/+iamd/+models/inputs2.xlsx
+++ b/+iamd/+models/inputs2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\Purdue MSAA\SoS\Project\ABM\+iamd\+models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8A143C-4B95-4448-A34E-57B34A2F62C3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D104D6F-9901-4510-A6FB-A2B650043D4F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="7350" tabRatio="442" activeTab="1" xr2:uid="{E29C2BC3-3FA1-4886-8308-3CCAE90EA738}"/>
   </bookViews>
@@ -658,7 +658,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +769,7 @@
         <v>250</v>
       </c>
       <c r="F2" s="20">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>7</v>
@@ -840,7 +840,7 @@
         <v>250</v>
       </c>
       <c r="F3" s="20">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="U3" s="6" t="s">
         <v>14</v>
@@ -878,7 +878,7 @@
         <v>250</v>
       </c>
       <c r="F4" s="20">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="U4" s="6" t="s">
         <v>15</v>

</xml_diff>